<commit_message>
make all image the same size
</commit_message>
<xml_diff>
--- a/monte_carlo/results/scenario2/heat_map.xlsx
+++ b/monte_carlo/results/scenario2/heat_map.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,7 +368,7 @@
     <col min="1" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>6.3963928524258504</v>
       </c>
@@ -385,7 +385,7 @@
         <v>1.1750750999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>52.161453240735497</v>
       </c>
@@ -402,7 +402,7 @@
         <v>1.305639</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>57.962710672824898</v>
       </c>
@@ -419,7 +419,7 @@
         <v>1.4507099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>64.581842124456102</v>
       </c>
@@ -436,7 +436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2.6617053238430799</v>
       </c>

</xml_diff>